<commit_message>
Added a new notebook for data viz
</commit_message>
<xml_diff>
--- a/excel/all_sql_queries.xlsx
+++ b/excel/all_sql_queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\OneDrive\Desktop\PROJECTS\Case Study - Sales Analysis 2019\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BF97BD-E910-4B57-A1DD-B8EB6A137736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1494033-9FB6-456D-AAC0-E7384A52F2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26805" yWindow="2805" windowWidth="21630" windowHeight="11250" activeTab="3" xr2:uid="{DDE6C5C2-414D-4A9C-AE95-6F24E27CA7A2}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>Total Revenue</t>
   </si>
@@ -208,12 +208,6 @@
   </si>
   <si>
     <t>Frequency</t>
-  </si>
-  <si>
-    <t>Total Sales</t>
-  </si>
-  <si>
-    <t>% of total sales</t>
   </si>
 </sst>
 </file>
@@ -223,10 +217,10 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,14 +229,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -267,28 +253,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -603,7 +583,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,7 +611,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,427 +664,327 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACF3399-031B-486A-A3D9-63850CE970E3}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>55</v>
+      <c r="C1" t="s">
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="2">
         <v>8032500</v>
       </c>
-      <c r="C2" s="6">
-        <f>B2/$B$21</f>
-        <v>0.23305888954884108</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="C2" s="3">
         <v>1700</v>
       </c>
-      <c r="E2" s="1">
+      <c r="D2" s="1">
         <v>4725</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2">
         <v>4792900</v>
       </c>
-      <c r="C3" s="6">
-        <f t="shared" ref="C3:C20" si="0">B3/$B$21</f>
-        <v>0.13906354829986187</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C3" s="3">
         <v>700</v>
       </c>
-      <c r="E3" s="1">
+      <c r="D3" s="1">
         <v>6847</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="2">
         <v>4127958.72000043</v>
       </c>
-      <c r="C4" s="6">
-        <f t="shared" si="0"/>
-        <v>0.11977061629464744</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="3">
         <v>999.99000000010506</v>
       </c>
-      <c r="E4" s="1">
+      <c r="D4" s="1">
         <v>4128</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="2">
         <v>3317400</v>
       </c>
-      <c r="C5" s="6">
-        <f t="shared" si="0"/>
-        <v>9.6252668557650217E-2</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="3">
         <v>600</v>
       </c>
-      <c r="E5" s="1">
+      <c r="D5" s="1">
         <v>5529</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="2">
         <v>2433147.61000014</v>
       </c>
-      <c r="C6" s="6">
-        <f t="shared" si="0"/>
-        <v>7.0596536582016714E-2</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="C6" s="3">
         <v>389.99000000002297</v>
       </c>
-      <c r="E6" s="1">
+      <c r="D6" s="1">
         <v>6239</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="2">
         <v>2352898.0800001002</v>
       </c>
-      <c r="C7" s="6">
-        <f t="shared" si="0"/>
-        <v>6.8268137410074523E-2</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7" s="3">
         <v>379.99000000001598</v>
       </c>
-      <c r="E7" s="1">
+      <c r="D7" s="1">
         <v>6192</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2">
         <v>2345550</v>
       </c>
-      <c r="C8" s="6">
-        <f t="shared" si="0"/>
-        <v>6.8054936617651315E-2</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="3">
         <v>150</v>
       </c>
-      <c r="E8" s="1">
+      <c r="D8" s="1">
         <v>15637</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2">
         <v>1443900</v>
       </c>
-      <c r="C9" s="6">
-        <f t="shared" si="0"/>
-        <v>4.1894021863625473E-2</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="C9" s="3">
         <v>300</v>
       </c>
-      <c r="E9" s="1">
+      <c r="D9" s="1">
         <v>4813</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2">
         <v>1342865.6999998901</v>
       </c>
-      <c r="C10" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8962563193924868E-2</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="C10" s="3">
         <v>99.989999999991795</v>
       </c>
-      <c r="E10" s="1">
+      <c r="D10" s="1">
         <v>13430</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>1131074.58999994</v>
       </c>
-      <c r="C11" s="6">
-        <f t="shared" si="0"/>
-        <v>3.2817552187027289E-2</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="C11" s="3">
         <v>149.98999999999199</v>
       </c>
-      <c r="E11" s="1">
+      <c r="D11" s="1">
         <v>7541</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2">
         <v>827200</v>
       </c>
-      <c r="C12" s="6">
-        <f t="shared" si="0"/>
-        <v>2.4000785986280901E-2</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="C12" s="3">
         <v>400</v>
       </c>
-      <c r="E12" s="1">
+      <c r="D12" s="1">
         <v>2068</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2">
         <v>453818.73999997502</v>
       </c>
-      <c r="C13" s="6">
-        <f t="shared" si="0"/>
-        <v>1.3167319215791895E-2</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="C13" s="3">
         <v>109.989999999994</v>
       </c>
-      <c r="E13" s="1">
+      <c r="D13" s="1">
         <v>4126</v>
       </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="2">
         <v>399600</v>
       </c>
-      <c r="C14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.1594190135538984E-2</v>
-      </c>
-      <c r="D14" s="3">
+      <c r="C14" s="3">
         <v>600</v>
       </c>
-      <c r="E14" s="1">
+      <c r="D14" s="1">
         <v>666</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="2">
         <v>387600</v>
       </c>
-      <c r="C15" s="6">
-        <f t="shared" si="0"/>
-        <v>1.124601625759487E-2</v>
-      </c>
-      <c r="D15" s="3">
+      <c r="C15" s="3">
         <v>600</v>
       </c>
-      <c r="E15" s="1">
+      <c r="D15" s="1">
         <v>646</v>
       </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2">
         <v>346376.55000013299</v>
       </c>
-      <c r="C16" s="6">
-        <f t="shared" si="0"/>
-        <v>1.004993888687079E-2</v>
-      </c>
-      <c r="D16" s="3">
+      <c r="C16" s="3">
         <v>14.9500000000057</v>
       </c>
-      <c r="E16" s="1">
+      <c r="D16" s="1">
         <v>23169</v>
       </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="2">
         <v>285975.45000010298</v>
       </c>
-      <c r="C17" s="6">
-        <f t="shared" si="0"/>
-        <v>8.2974317852790684E-3</v>
-      </c>
-      <c r="D17" s="3">
+      <c r="C17" s="3">
         <v>11.9500000000043</v>
       </c>
-      <c r="E17" s="1">
+      <c r="D17" s="1">
         <v>23931</v>
       </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="2">
         <v>246082.75999995199</v>
       </c>
-      <c r="C18" s="6">
-        <f t="shared" si="0"/>
-        <v>7.1399657370311573E-3</v>
-      </c>
-      <c r="D18" s="3">
+      <c r="C18" s="3">
         <v>11.9899999999976</v>
       </c>
-      <c r="E18" s="1">
+      <c r="D18" s="1">
         <v>20524</v>
       </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="2">
         <v>106041.59999995401</v>
       </c>
-      <c r="C19" s="6">
-        <f t="shared" si="0"/>
-        <v>3.076742924615209E-3</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="C19" s="3">
         <v>3.8399999999983501</v>
       </c>
-      <c r="E19" s="1">
+      <c r="D19" s="1">
         <v>27615</v>
       </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="2">
         <v>92648.140000015497</v>
       </c>
-      <c r="C20" s="6">
-        <f t="shared" si="0"/>
-        <v>2.6881385156762123E-3</v>
-      </c>
-      <c r="D20" s="3">
+      <c r="C20" s="3">
         <v>2.9900000000004998</v>
       </c>
-      <c r="E20" s="1">
+      <c r="D20" s="1">
         <v>30986</v>
       </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="4">
-        <f>SUM(B2:B20)</f>
-        <v>34465537.940000638</v>
-      </c>
-      <c r="C21" s="6">
-        <f>SUM(C2:C20)</f>
-        <v>0.99999999999999989</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="4">
-        <f>SUM(B8,B10,B16:B18)</f>
-        <v>4566850.4600000782</v>
-      </c>
-      <c r="C22" s="6">
-        <f>B22/B21</f>
-        <v>0.13250483622075721</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="4">
-        <f>B2</f>
-        <v>8032500</v>
-      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>